<commit_message>
finished master file saving
</commit_message>
<xml_diff>
--- a/excel_templates/master-template.xlsx
+++ b/excel_templates/master-template.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorverra/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorverra/PycharmProjects/CAN-Injury-Tracker/excel_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25620847-F436-3844-B488-683D3853D921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC629A3-B77A-5346-97F7-35045EAE06A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{2EE6441C-3266-2C4F-BE42-E3E4848A3618}"/>
+    <workbookView xWindow="1160" yWindow="1060" windowWidth="27640" windowHeight="16940" xr2:uid="{2EE6441C-3266-2C4F-BE42-E3E4848A3618}"/>
   </bookViews>
   <sheets>
-    <sheet name="MasterData" sheetId="1" r:id="rId1"/>
+    <sheet name="Master Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,16 +41,10 @@
     <t>Calculations</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t># of injuries</t>
   </si>
   <si>
     <t>Average Size</t>
-  </si>
-  <si>
-    <t>LARGEST SIZE</t>
   </si>
   <si>
     <t>Bruise</t>
@@ -78,6 +72,12 @@
   </si>
   <si>
     <t>Comparisons (with last check)</t>
+  </si>
+  <si>
+    <t>Largest Size</t>
+  </si>
+  <si>
+    <t>Date + Time</t>
   </si>
 </sst>
 </file>
@@ -331,27 +331,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -369,36 +349,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -424,131 +374,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -885,7 +715,7 @@
   <dimension ref="B1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -900,7 +730,7 @@
     <row r="1" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:13" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>0</v>
@@ -909,53 +739,53 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="5"/>
       <c r="L2" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M2" s="5"/>
     </row>
     <row r="3" spans="2:13" ht="32" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="F3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="8" t="s">
+      <c r="K3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="11" t="s">
         <v>6</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.2">
@@ -10939,23 +10769,23 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="L4:M1000">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>AND(ISNUMBER(L4), L4&gt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>AND(ISNUMBER(L4), L4&lt;0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>AND(ISNUMBER(L4), L4=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="L1001:M2000">
-    <cfRule type="expression" dxfId="10" priority="5">
-      <formula>AND(ISNUMBER(F1002), F1002&gt;0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>AND(ISNUMBER(F1002), F1002&lt;0)</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L4:M1000">
-    <cfRule type="expression" dxfId="7" priority="3">
-      <formula>AND(ISNUMBER(L4), L4=0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
-      <formula>AND(ISNUMBER(L4), L4&lt;0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="1">
-      <formula>AND(ISNUMBER(L4), L4&gt;0)</formula>
+    <cfRule type="expression" dxfId="0" priority="5">
+      <formula>AND(ISNUMBER(F1002), F1002&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>